<commit_message>
Warnings, arreglos y entrenamiento bien, docker
</commit_message>
<xml_diff>
--- a/entrenamiento/resultados/Aproximacion2.xlsx
+++ b/entrenamiento/resultados/Aproximacion2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive - Universidade da Coruña\UDC4\TFG\ComunicELA-tfg\entrenamiento\resultados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udcgal-my.sharepoint.com/personal/pablo_paramo_telle_udc_es/Documents/UDC4/TFG/ComunicELA-tfg/entrenamiento/resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA6E94-DA07-4A47-99E0-6EB6066B0DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4121EB-B7BD-453F-A6C6-EDBD70116562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Modelo</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Se escoge el Dataset de imagenes 15-15-15 y el modelo 3-3 de las terceras observaciones para la fusionNet</t>
+  </si>
+  <si>
+    <t>18-15-15-15</t>
+  </si>
+  <si>
+    <t>34-15-15-15</t>
   </si>
 </sst>
 </file>
@@ -105,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,14 +134,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,9 +726,43 @@
         <v>7.8174374089508947E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2.2425920290000002E-2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1.7141856309999998E-2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.17179384719999999</v>
+      </c>
+      <c r="E23" s="3">
+        <v>7.4130151170000005E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>2.09739276057321E-2</v>
+      </c>
+      <c r="C24">
+        <v>1.48236300644138E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.16989446888458901</v>
+      </c>
+      <c r="E24">
+        <v>6.6298697244129096E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mejoras código limpieza y nuevas aprox
</commit_message>
<xml_diff>
--- a/entrenamiento/resultados/Aproximacion2.xlsx
+++ b/entrenamiento/resultados/Aproximacion2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udcgal-my.sharepoint.com/personal/pablo_paramo_telle_udc_es/Documents/UDC4/TFG/ComunicELA-tfg/entrenamiento/resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4121EB-B7BD-453F-A6C6-EDBD70116562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3B4121EB-B7BD-453F-A6C6-EDBD70116562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B74A472D-CAC1-4F83-8A4F-6845A69A80B1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34485" yWindow="1110" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,13 +76,13 @@
     <t>4-4-15-35-15</t>
   </si>
   <si>
-    <t>Se escoge el Dataset de imagenes 15-15-15 y el modelo 3-3 de las terceras observaciones para la fusionNet</t>
-  </si>
-  <si>
     <t>18-15-15-15</t>
   </si>
   <si>
     <t>34-15-15-15</t>
+  </si>
+  <si>
+    <t>Se escoge el Dataset de imagenes 15-15-15 y el modelo 3-3 de las terceras observaciones para la ResNet</t>
   </si>
 </sst>
 </file>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,12 +728,12 @@
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3">
         <v>2.2425920290000002E-2</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>2.09739276057321E-2</v>

</xml_diff>